<commit_message>
Updated Test Cases for Rooted In Demo
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SingleLine.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SingleLine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3A36EEC5-7779-4156-8934-1A5BB7B6B59F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{DFF1173C-844C-4637-87F2-AEE117D48D14}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="AddHeader" r:id="rId1" sheetId="14"/>
     <sheet name="AddLine" r:id="rId2" sheetId="15"/>
     <sheet name="InventoryQuantity" r:id="rId3" sheetId="12"/>
-    <sheet name="SOFulfillment" r:id="rId4" sheetId="16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
-  <si>
-    <t>Product</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Unit Price</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Line Number</t>
   </si>
   <si>
@@ -69,9 +62,6 @@
     <t>a1X5f000003jRuy</t>
   </si>
   <si>
-    <t>IsSerial</t>
-  </si>
-  <si>
     <t>CustomerName</t>
   </si>
   <si>
@@ -81,19 +71,25 @@
     <t>ProductName</t>
   </si>
   <si>
-    <t>53.0</t>
-  </si>
-  <si>
-    <t>69.0</t>
-  </si>
-  <si>
     <t>QtyOrdered</t>
   </si>
   <si>
-    <t>68.0</t>
-  </si>
-  <si>
     <t>67.0</t>
+  </si>
+  <si>
+    <t>66.0</t>
+  </si>
+  <si>
+    <t>65.0</t>
+  </si>
+  <si>
+    <t>64.0</t>
+  </si>
+  <si>
+    <t>63.0</t>
+  </si>
+  <si>
+    <t>62.0</t>
   </si>
 </sst>
 </file>
@@ -103,19 +99,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -129,13 +119,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -248,24 +231,22 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="6" numFmtId="49" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="10" numFmtId="49" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="10" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="12" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="14" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="12" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -548,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28DC5EA-FDB2-4037-A650-5A7807A76B42}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,13 +539,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>11</v>
+      <c r="A1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -589,22 +570,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -626,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7667096-5FA7-42EB-ACDF-85A64908BEC3}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -640,76 +621,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E98237-5B33-4FA7-92DA-167DD1319B66}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated SO Fulfillment Test Cases
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SingleLine.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SingleLine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{DFF1173C-844C-4637-87F2-AEE117D48D14}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{C8C0DC26-0514-47F1-A031-6D36738474BF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="2" windowHeight="15840" windowWidth="29040" xWindow="20370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-1020"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" r:id="rId1" sheetId="14"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Unit Price</t>
   </si>
@@ -71,25 +71,25 @@
     <t>ProductName</t>
   </si>
   <si>
-    <t>QtyOrdered</t>
-  </si>
-  <si>
-    <t>67.0</t>
-  </si>
-  <si>
-    <t>66.0</t>
-  </si>
-  <si>
-    <t>65.0</t>
-  </si>
-  <si>
-    <t>64.0</t>
-  </si>
-  <si>
     <t>63.0</t>
   </si>
   <si>
     <t>62.0</t>
+  </si>
+  <si>
+    <t>Order Quantity</t>
+  </si>
+  <si>
+    <t>Automation5501-2 (Mfg-LotYes)</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>79.0</t>
+  </si>
+  <si>
+    <t>78.0</t>
   </si>
 </sst>
 </file>
@@ -99,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,42 +119,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -201,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -218,20 +182,11 @@
     <border>
       <bottom style="thin"/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -239,14 +194,8 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="10" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="12" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -529,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28DC5EA-FDB2-4037-A650-5A7807A76B42}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,10 +504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513CC44F-3165-4623-A12A-9D782A7314E2}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -595,6 +544,20 @@
       </c>
       <c r="D2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7667096-5FA7-42EB-ACDF-85A64908BEC3}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>